<commit_message>
More sequence plotter edits
</commit_message>
<xml_diff>
--- a/examples/q2d_rf_sequence.xlsx
+++ b/examples/q2d_rf_sequence.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\colin\Documents\GitHub\chip-lab\ChiPyLab\examples\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{554B4F1D-F161-4F72-A9D6-45A7814E796D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B5CC71B0-F950-495C-853A-14352B73E7DB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="12220" xr2:uid="{D818C0C5-7768-4858-97A0-2DC1B457CA77}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="22">
   <si>
     <t>segments</t>
   </si>
@@ -44,24 +44,12 @@
     <t>times</t>
   </si>
   <si>
-    <t>set point</t>
-  </si>
-  <si>
-    <t>pi pulse</t>
-  </si>
-  <si>
     <t>wait</t>
   </si>
   <si>
     <t>jump</t>
   </si>
   <si>
-    <t>SSI</t>
-  </si>
-  <si>
-    <t>20ms</t>
-  </si>
-  <si>
     <t>10ms</t>
   </si>
   <si>
@@ -101,12 +89,6 @@
     <t>160us</t>
   </si>
   <si>
-    <t>pause</t>
-  </si>
-  <si>
-    <t>20us</t>
-  </si>
-  <si>
     <t>sweep</t>
   </si>
   <si>
@@ -114,6 +96,12 @@
   </si>
   <si>
     <t>scale</t>
+  </si>
+  <si>
+    <t>π pulse</t>
+  </si>
+  <si>
+    <t>9ms</t>
   </si>
 </sst>
 </file>
@@ -485,10 +473,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{012E0891-FB82-47F4-804A-8621778D1A0B}">
-  <dimension ref="A1:G10"/>
+  <dimension ref="A1:G12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G4" sqref="G4"/>
+      <selection activeCell="B10" sqref="B10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -509,157 +497,161 @@
         <v>1</v>
       </c>
       <c r="C1" t="s">
-        <v>25</v>
+        <v>19</v>
       </c>
       <c r="D1" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="E1" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="F1" t="s">
-        <v>14</v>
+        <v>10</v>
       </c>
       <c r="G1" t="s">
-        <v>15</v>
+        <v>11</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A2" t="s">
-        <v>2</v>
-      </c>
-      <c r="B2" t="s">
-        <v>7</v>
-      </c>
       <c r="C2">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D2">
         <v>0</v>
       </c>
       <c r="E2" t="s">
-        <v>19</v>
+        <v>15</v>
       </c>
       <c r="F2">
         <v>198</v>
       </c>
       <c r="G2" t="s">
-        <v>19</v>
+        <v>15</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
-        <v>3</v>
+        <v>20</v>
       </c>
       <c r="B3" t="s">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="C3">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="D3">
         <v>2</v>
       </c>
       <c r="E3" t="s">
-        <v>19</v>
+        <v>15</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
+        <v>2</v>
+      </c>
+      <c r="B4" t="s">
+        <v>16</v>
+      </c>
+      <c r="C4">
         <v>4</v>
-      </c>
-      <c r="B4" t="s">
-        <v>20</v>
-      </c>
-      <c r="C4">
-        <v>16</v>
       </c>
       <c r="D4">
         <v>0</v>
       </c>
       <c r="E4" t="s">
-        <v>19</v>
+        <v>15</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
-        <v>17</v>
+        <v>13</v>
       </c>
       <c r="B5" t="s">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="C5">
-        <v>12</v>
+        <v>3</v>
       </c>
       <c r="E5" t="s">
-        <v>18</v>
+        <v>14</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A6" t="s">
-        <v>21</v>
-      </c>
-      <c r="B6" t="s">
-        <v>22</v>
-      </c>
       <c r="C6">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="B7" t="s">
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="C7">
-        <v>1</v>
+        <v>0.5</v>
       </c>
       <c r="F7">
         <v>210</v>
       </c>
       <c r="G7" t="s">
-        <v>16</v>
+        <v>12</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
-        <v>24</v>
+        <v>18</v>
       </c>
       <c r="B8" t="s">
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="C8">
-        <v>20</v>
+        <v>4</v>
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A9" t="s">
-        <v>23</v>
-      </c>
-      <c r="B9" t="s">
-        <v>8</v>
-      </c>
       <c r="C9">
-        <v>20</v>
-      </c>
-      <c r="F9">
-        <v>209</v>
-      </c>
-      <c r="G9" t="s">
-        <v>16</v>
+        <v>1</v>
+      </c>
+      <c r="D9">
+        <v>10</v>
+      </c>
+      <c r="E9" t="s">
+        <v>12</v>
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
-        <v>6</v>
+        <v>17</v>
       </c>
       <c r="B10" t="s">
-        <v>8</v>
+        <v>21</v>
       </c>
       <c r="C10">
-        <v>20</v>
+        <v>2.5</v>
+      </c>
+      <c r="F10">
+        <v>209</v>
+      </c>
+      <c r="G10" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="C11">
+        <v>1</v>
+      </c>
+      <c r="D11">
+        <v>0</v>
+      </c>
+      <c r="E11" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="C12">
+        <v>1</v>
       </c>
     </row>
   </sheetData>

</xml_diff>